<commit_message>
Added STM32 Project files: target_device, link_layer
</commit_message>
<xml_diff>
--- a/Protocol/FrameCalculations.xlsx
+++ b/Protocol/FrameCalculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="14625"/>
+    <workbookView xWindow="120" yWindow="165" windowWidth="28515" windowHeight="14565"/>
   </bookViews>
   <sheets>
     <sheet name="FrameDefinition" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
   <si>
     <t>Flash Size</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Time[m]</t>
+  </si>
+  <si>
+    <t>Flash ACK Request</t>
   </si>
 </sst>
 </file>
@@ -201,7 +204,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -412,22 +415,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -444,7 +432,22 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="40 % - Akzent1" xfId="3" builtinId="31"/>
@@ -752,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH23"/>
+  <dimension ref="A1:AH25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,42 +773,42 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="20"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -813,7 +816,7 @@
       </c>
       <c r="B2">
         <f>B1*1000</f>
-        <v>16000</v>
+        <v>8000</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -912,7 +915,7 @@
       </c>
       <c r="B3">
         <f>B2*1000</f>
-        <v>16000000</v>
+        <v>8000000</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -927,7 +930,7 @@
       </c>
       <c r="B4">
         <f>B3/8</f>
-        <v>2000000</v>
+        <v>1000000</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -935,45 +938,45 @@
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="5" t="s">
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="5"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="21"/>
+      <c r="AB4" s="21"/>
+      <c r="AC4" s="21"/>
+      <c r="AD4" s="21"/>
+      <c r="AE4" s="21"/>
+      <c r="AF4" s="21"/>
+      <c r="AG4" s="21"/>
+      <c r="AH4" s="21"/>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <f>ROUNDUP(LOG((B4+1),2)-1,0)</f>
+        <f>ROUNDUP(LOG((B4+1),2),0)</f>
         <v>20</v>
       </c>
       <c r="C5" t="s">
@@ -982,26 +985,26 @@
       <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="9" t="s">
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1012,10 +1015,10 @@
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="4">
         <v>1</v>
       </c>
     </row>
@@ -1035,127 +1038,147 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <f>BaudRate</f>
         <v>1000</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14">
-        <f>MessageTable!D2</f>
-        <v>4000</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>4000</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>52</v>
       </c>
-      <c r="B15">
-        <f>B14*8/1000</f>
+      <c r="B16">
+        <f>B15*8/1000</f>
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="16">
+        <f>BusDefinition!B15</f>
+        <v>61.8125</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B19" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C19" s="18" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>100</v>
-      </c>
-      <c r="B18">
-        <f>A18/$B$15</f>
-        <v>3.125</v>
-      </c>
-      <c r="C18" s="24">
-        <f>B18/60</f>
-        <v>5.2083333333333336E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>250</v>
-      </c>
-      <c r="B19" s="10">
-        <f t="shared" ref="B19:B23" si="0">A19/$B$15</f>
-        <v>7.8125</v>
-      </c>
-      <c r="C19" s="24">
-        <f t="shared" ref="C19:C23" si="1">B19/60</f>
-        <v>0.13020833333333334</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>100</v>
+      </c>
+      <c r="B20" s="19">
+        <f>A20/$B$16</f>
+        <v>3.125</v>
+      </c>
+      <c r="C20" s="19">
+        <f>B20/60</f>
+        <v>5.2083333333333336E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>250</v>
+      </c>
+      <c r="B21" s="19">
+        <f t="shared" ref="B21:B25" si="0">A21/$B$16</f>
+        <v>7.8125</v>
+      </c>
+      <c r="C21" s="19">
+        <f t="shared" ref="C21:C25" si="1">B21/60</f>
+        <v>0.13020833333333334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>500</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B22" s="19">
         <f t="shared" si="0"/>
         <v>15.625</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C22" s="19">
         <f t="shared" si="1"/>
         <v>0.26041666666666669</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>1000</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B23" s="19">
         <f t="shared" si="0"/>
         <v>31.25</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C23" s="19">
         <f t="shared" si="1"/>
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>2000</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B24" s="19">
         <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C24" s="19">
         <f t="shared" si="1"/>
         <v>1.0416666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>5000</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B25" s="19">
         <f t="shared" si="0"/>
         <v>156.25</v>
       </c>
-      <c r="C23" s="24">
+      <c r="C25" s="19">
         <f t="shared" si="1"/>
         <v>2.6041666666666665</v>
       </c>
@@ -1175,15 +1198,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="10"/>
+    <col min="1" max="1" width="11.42578125" style="5"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -1193,120 +1216,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="5">
         <v>64</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="5">
+        <f>FrameDefinition!B15</f>
         <v>4000</v>
       </c>
-      <c r="E2" s="10">
-        <f>ROUNDUP(C2/MaxChunkSize,0)</f>
+      <c r="E2" s="5">
+        <f>MAX(ROUNDUP(C2/MaxChunkSize,0),1)</f>
         <v>1</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="5">
         <f>((E2-1)*(MessageOverhead+MaxChunkSize+FLOOR((StuffingOverhead+MaxChunkSize)/StuffingAfter,1))) + (MessageOverhead+IF(C2=64,64,MOD(C2,MaxChunkSize))+FLOOR((StuffingOverhead+IF(C2=64,64,MOD(C2,MaxChunkSize)))/StuffingAfter,1))</f>
         <v>151</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="5">
         <f>F2*D2*A2</f>
         <v>604000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+    <row r="3" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="B3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="5">
         <v>0</v>
       </c>
-      <c r="D3" s="10">
-        <f>D2/10</f>
-        <v>400</v>
-      </c>
-      <c r="E3" s="10">
+      <c r="D3" s="5">
+        <f>D2/64</f>
+        <v>62.5</v>
+      </c>
+      <c r="E3" s="5">
         <f>MAX(ROUNDUP(C3/MaxChunkSize,0),1)</f>
         <v>1</v>
       </c>
-      <c r="F3" s="10">
-        <f>((E3-1)*(MessageOverhead+MaxChunkSize+FLOOR((StuffingOverhead+MaxChunkSize)/StuffingAfter,1))) + (MessageOverhead+MOD(C3,MaxChunkSize)+FLOOR((StuffingOverhead+MOD(C3,MaxChunkSize))/StuffingAfter,1))</f>
+      <c r="F3" s="5">
+        <f>((E3-1)*(MessageOverhead+MaxChunkSize+FLOOR((StuffingOverhead+MaxChunkSize)/StuffingAfter,1))) + (MessageOverhead+IF(C3=64,64,MOD(C3,MaxChunkSize))+FLOOR((StuffingOverhead+IF(C3=64,64,MOD(C3,MaxChunkSize)))/StuffingAfter,1))</f>
         <v>75</v>
       </c>
-      <c r="G3" s="10">
-        <f>F3*D3*A3</f>
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="18" t="s">
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G4" si="0">F3*D3*A3</f>
+        <v>4687.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="5">
+        <v>64</v>
+      </c>
+      <c r="D4" s="5">
+        <f>D2/64</f>
+        <v>62.5</v>
+      </c>
+      <c r="E4" s="5">
+        <f>MAX(ROUNDUP(C4/MaxChunkSize,0),1)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <f>((E4-1)*(MessageOverhead+MaxChunkSize+FLOOR((StuffingOverhead+MaxChunkSize)/StuffingAfter,1))) + (MessageOverhead+IF(C4=64,64,MOD(C4,MaxChunkSize))+FLOOR((StuffingOverhead+IF(C4=64,64,MOD(C4,MaxChunkSize)))/StuffingAfter,1))</f>
+        <v>151</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
+        <v>9437.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="10">
-        <f>SUM(G2:G5)</f>
-        <v>634000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F7" t="s">
+      <c r="G7" s="5">
+        <f>SUM(G2:G6)</f>
+        <v>618125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G8" s="17">
         <f>BusDefinition!B15</f>
-        <v>63.4</v>
-      </c>
-      <c r="H7" t="s">
+        <v>61.8125</v>
+      </c>
+      <c r="H8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1336,192 +1387,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="10">
         <v>32</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="10">
         <v>6</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10">
         <v>16</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="10">
         <v>2</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="11">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="15">
         <v>1000</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="5">
         <f>B4+C4+D4+F4+G4+H4</f>
         <v>64</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="5">
         <v>5</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="5">
         <f>B4+C4+D4+F4</f>
         <v>55</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="5">
         <v>64</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="10">
-        <f>MessageTable!G6</f>
-        <v>634000</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="5">
+        <f>MessageTable!G7</f>
+        <v>618125</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="16">
         <f>B14/(BaudRate*1000)*100</f>
-        <v>63.4</v>
-      </c>
-      <c r="C15" s="10" t="s">
+        <v>61.8125</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>